<commit_message>
suite admin et securisation
</commit_message>
<xml_diff>
--- a/src/fichiers/csv_adherents/adherents.xlsx
+++ b/src/fichiers/csv_adherents/adherents.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="55">
   <si>
     <t>ADHERENTS SAISON SPORTIVE 2021-2022</t>
   </si>
@@ -144,6 +144,24 @@
   </si>
   <si>
     <t>gq</t>
+  </si>
+  <si>
+    <t>sdivhdsiof</t>
+  </si>
+  <si>
+    <t>sdifndsif</t>
+  </si>
+  <si>
+    <t>io</t>
+  </si>
+  <si>
+    <t>djahit</t>
+  </si>
+  <si>
+    <t>ihd</t>
+  </si>
+  <si>
+    <t>okkk</t>
   </si>
   <si>
     <t>Total</t>
@@ -956,10 +974,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:X21"/>
+  <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="W15" sqref="W15"/>
+      <selection activeCell="W19" sqref="W19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="true" defaultRowHeight="22.5" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1465,7 +1483,7 @@
       <c r="X13" s="8"/>
     </row>
     <row r="14" spans="1:24">
-      <c r="A14" s="27">
+      <c r="A14" s="8">
         <v>3</v>
       </c>
       <c r="B14" s="18" t="s">
@@ -1507,202 +1525,368 @@
       <c r="W14" s="26"/>
       <c r="X14" s="8"/>
     </row>
-    <row r="15" spans="1:24" customHeight="1" ht="30">
-      <c r="B15" s="54"/>
-      <c r="C15" s="28" t="s">
+    <row r="15" spans="1:24">
+      <c r="A15" s="8">
+        <v>4</v>
+      </c>
+      <c r="B15" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="30">
-        <f>SUM(D12:D14)</f>
-        <v>0</v>
-      </c>
-      <c r="E15" s="30">
-        <f>SUM(E12:E14)</f>
-        <v>450</v>
-      </c>
-      <c r="F15" s="28">
-        <f>SUM(F12:F14)</f>
-        <v>1</v>
-      </c>
-      <c r="G15" s="31"/>
-      <c r="H15" s="28">
-        <f>SUM(H12:H14)</f>
-        <v>2</v>
-      </c>
-      <c r="I15" s="30">
-        <f>SUM(I12:I14)</f>
-        <v>0</v>
-      </c>
-      <c r="J15" s="30">
-        <f>SUM(J12:J14)</f>
-        <v>0</v>
-      </c>
-      <c r="K15" s="32">
-        <f>SUM(K12:K14)</f>
-        <v>0</v>
-      </c>
-      <c r="L15" s="30">
-        <f>SUM(L12:L14)</f>
-        <v>0</v>
-      </c>
-      <c r="M15" s="29">
-        <f>SUM(M12:M14)</f>
-        <v>0</v>
-      </c>
-      <c r="N15" s="29">
-        <f>SUM(N12:N14)</f>
-        <v>0</v>
-      </c>
-      <c r="O15" s="29">
-        <f>SUM(O12:O14)</f>
-        <v>0</v>
-      </c>
-      <c r="P15" s="29">
-        <f>SUM(P12:P14)</f>
-        <v>0</v>
-      </c>
-      <c r="Q15" s="32">
-        <f>SUM(Q12:Q14)</f>
-        <v>0</v>
-      </c>
-      <c r="R15" s="33">
-        <f>SUM(R12:R14)</f>
-        <v>0</v>
-      </c>
-      <c r="S15" s="33">
-        <f>SUM(S12:S14)</f>
-        <v>0</v>
-      </c>
-      <c r="T15" s="34">
-        <f>SUM(T12:T14)</f>
-        <v>2</v>
-      </c>
-      <c r="U15" s="35">
-        <f>SUM(U12:U14)</f>
-        <v>0</v>
-      </c>
-      <c r="V15" s="34">
-        <f>SUM(V12:V14)</f>
-        <v>1</v>
-      </c>
-      <c r="W15" s="55">
-        <f>SUM(W12:W14)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24" customHeight="1" ht="30">
-      <c r="D16" s="36">
-        <f>SUM(D15:E15)</f>
-        <v>450</v>
-      </c>
-      <c r="E16" s="37"/>
-      <c r="O16" s="38">
-        <f>SUM(O15:P15)</f>
-        <v>0</v>
-      </c>
-      <c r="P16" s="37"/>
-    </row>
-    <row r="17" spans="1:24" customHeight="1" ht="19.5">
-      <c r="B17" s="39" t="s">
+      <c r="C15" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="40"/>
-      <c r="D17" s="41">
-        <f>D16</f>
-        <v>450</v>
-      </c>
-      <c r="E17" s="42"/>
-      <c r="J17" s="44" t="s">
+      <c r="D15" s="20">
+        <v>0</v>
+      </c>
+      <c r="E15" s="21">
+        <f>E11</f>
+        <v>150</v>
+      </c>
+      <c r="F15" s="18"/>
+      <c r="G15" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H15" s="19">
+        <v>1</v>
+      </c>
+      <c r="I15" s="20"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="17"/>
+      <c r="P15" s="21"/>
+      <c r="Q15" s="22"/>
+      <c r="R15" s="20"/>
+      <c r="S15" s="21"/>
+      <c r="T15" s="23">
+        <v>1</v>
+      </c>
+      <c r="U15" s="24"/>
+      <c r="V15" s="25"/>
+      <c r="W15" s="26"/>
+      <c r="X15" s="8"/>
+    </row>
+    <row r="16" spans="1:24">
+      <c r="A16" s="8">
+        <v>5</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="K17" s="44"/>
-      <c r="L17" s="45">
-        <f>SUM(L15:P15)</f>
-        <v>0</v>
-      </c>
-      <c r="M17" s="46"/>
-      <c r="N17" s="46"/>
-      <c r="O17" s="46"/>
-      <c r="P17" s="46"/>
-      <c r="R17" s="47">
-        <f>SUM(R15:S15)</f>
-        <v>0</v>
-      </c>
-      <c r="S17" s="47"/>
-      <c r="T17" s="48">
-        <f>SUM(T15+V15)</f>
+      <c r="D16" s="20">
+        <v>0</v>
+      </c>
+      <c r="E16" s="21">
+        <f>E11</f>
+        <v>150</v>
+      </c>
+      <c r="F16" s="18">
+        <v>1</v>
+      </c>
+      <c r="G16" s="8"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="21"/>
+      <c r="Q16" s="22"/>
+      <c r="R16" s="20"/>
+      <c r="S16" s="21"/>
+      <c r="T16" s="23">
+        <v>1</v>
+      </c>
+      <c r="U16" s="24"/>
+      <c r="V16" s="25"/>
+      <c r="W16" s="26"/>
+      <c r="X16" s="8"/>
+    </row>
+    <row r="17" spans="1:24">
+      <c r="A17" s="8">
+        <v>6</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="20">
+        <v>0</v>
+      </c>
+      <c r="E17" s="21">
+        <f>E11</f>
+        <v>150</v>
+      </c>
+      <c r="F17" s="18">
+        <v>1</v>
+      </c>
+      <c r="G17" s="8"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="17"/>
+      <c r="O17" s="17"/>
+      <c r="P17" s="21"/>
+      <c r="Q17" s="22"/>
+      <c r="R17" s="20"/>
+      <c r="S17" s="21"/>
+      <c r="T17" s="23">
+        <v>1</v>
+      </c>
+      <c r="U17" s="24"/>
+      <c r="V17" s="25"/>
+      <c r="W17" s="26"/>
+      <c r="X17" s="8"/>
+    </row>
+    <row r="18" spans="1:24">
+      <c r="A18" s="27">
+        <v>7</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="20">
+        <v>0</v>
+      </c>
+      <c r="E18" s="21">
+        <f>E11</f>
+        <v>150</v>
+      </c>
+      <c r="F18" s="18">
+        <v>1</v>
+      </c>
+      <c r="G18" s="8"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="17"/>
+      <c r="O18" s="17"/>
+      <c r="P18" s="21"/>
+      <c r="Q18" s="22"/>
+      <c r="R18" s="20"/>
+      <c r="S18" s="21"/>
+      <c r="T18" s="23">
+        <v>1</v>
+      </c>
+      <c r="U18" s="24"/>
+      <c r="V18" s="25"/>
+      <c r="W18" s="26"/>
+      <c r="X18" s="8"/>
+    </row>
+    <row r="19" spans="1:24" customHeight="1" ht="30">
+      <c r="B19" s="54"/>
+      <c r="C19" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="30">
+        <f>SUM(D12:D18)</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="30">
+        <f>SUM(E12:E18)</f>
+        <v>1050</v>
+      </c>
+      <c r="F19" s="28">
+        <f>SUM(F12:F18)</f>
+        <v>4</v>
+      </c>
+      <c r="G19" s="31"/>
+      <c r="H19" s="28">
+        <f>SUM(H12:H18)</f>
         <v>3</v>
       </c>
-      <c r="U17" s="48"/>
-      <c r="V17" s="49">
-        <f>SUM(U15+W15)</f>
-        <v>0</v>
-      </c>
-      <c r="W17" s="49"/>
-    </row>
-    <row r="18" spans="1:24" customHeight="1" ht="19.5">
-      <c r="B18" s="39" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" s="40"/>
-      <c r="D18" s="41">
-        <f>K15</f>
-        <v>0</v>
-      </c>
-      <c r="E18" s="42"/>
-      <c r="J18" s="44"/>
-      <c r="K18" s="44"/>
-      <c r="L18" s="46"/>
-      <c r="M18" s="46"/>
-      <c r="N18" s="46"/>
-      <c r="O18" s="46"/>
-      <c r="P18" s="46"/>
-      <c r="R18" s="47"/>
-      <c r="S18" s="47"/>
-      <c r="T18" s="48"/>
-      <c r="U18" s="48"/>
-      <c r="V18" s="49"/>
-      <c r="W18" s="49"/>
-    </row>
-    <row r="19" spans="1:24" customHeight="1" ht="19.5">
-      <c r="B19" s="39" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="41">
-        <f>D17-D18</f>
-        <v>450</v>
-      </c>
-      <c r="E19" s="42"/>
-      <c r="T19" s="43">
-        <f>SUM(T17:W18)</f>
-        <v>3</v>
-      </c>
-      <c r="U19" s="43"/>
-      <c r="V19" s="43"/>
-      <c r="W19" s="43"/>
-    </row>
-    <row r="20" spans="1:24" customHeight="1" ht="19.5">
-      <c r="N20" s="50">
-        <f>SUM(Q15+K15)</f>
-        <v>0</v>
-      </c>
-      <c r="O20" s="51"/>
-      <c r="T20" s="43"/>
-      <c r="U20" s="43"/>
-      <c r="V20" s="43"/>
-      <c r="W20" s="43"/>
+      <c r="I19" s="30">
+        <f>SUM(I12:I18)</f>
+        <v>0</v>
+      </c>
+      <c r="J19" s="30">
+        <f>SUM(J12:J18)</f>
+        <v>0</v>
+      </c>
+      <c r="K19" s="32">
+        <f>SUM(K12:K18)</f>
+        <v>0</v>
+      </c>
+      <c r="L19" s="30">
+        <f>SUM(L12:L18)</f>
+        <v>0</v>
+      </c>
+      <c r="M19" s="29">
+        <f>SUM(M12:M18)</f>
+        <v>0</v>
+      </c>
+      <c r="N19" s="29">
+        <f>SUM(N12:N18)</f>
+        <v>0</v>
+      </c>
+      <c r="O19" s="29">
+        <f>SUM(O12:O18)</f>
+        <v>0</v>
+      </c>
+      <c r="P19" s="29">
+        <f>SUM(P12:P18)</f>
+        <v>0</v>
+      </c>
+      <c r="Q19" s="32">
+        <f>SUM(Q12:Q18)</f>
+        <v>0</v>
+      </c>
+      <c r="R19" s="33">
+        <f>SUM(R12:R18)</f>
+        <v>0</v>
+      </c>
+      <c r="S19" s="33">
+        <f>SUM(S12:S18)</f>
+        <v>0</v>
+      </c>
+      <c r="T19" s="34">
+        <f>SUM(T12:T18)</f>
+        <v>6</v>
+      </c>
+      <c r="U19" s="35">
+        <f>SUM(U12:U18)</f>
+        <v>0</v>
+      </c>
+      <c r="V19" s="34">
+        <f>SUM(V12:V18)</f>
+        <v>1</v>
+      </c>
+      <c r="W19" s="55">
+        <f>SUM(W12:W18)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" customHeight="1" ht="30">
+      <c r="D20" s="36">
+        <f>SUM(D19:E19)</f>
+        <v>1050</v>
+      </c>
+      <c r="E20" s="37"/>
+      <c r="O20" s="38">
+        <f>SUM(O19:P19)</f>
+        <v>0</v>
+      </c>
+      <c r="P20" s="37"/>
     </row>
     <row r="21" spans="1:24" customHeight="1" ht="19.5">
-      <c r="I21" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="J21" s="53">
-        <f>SUM(D16-N20)</f>
-        <v>450</v>
-      </c>
-      <c r="N21" s="51"/>
-      <c r="O21" s="51"/>
+      <c r="B21" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="40"/>
+      <c r="D21" s="41">
+        <f>D20</f>
+        <v>1050</v>
+      </c>
+      <c r="E21" s="42"/>
+      <c r="J21" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="K21" s="44"/>
+      <c r="L21" s="45">
+        <f>SUM(L19:P19)</f>
+        <v>0</v>
+      </c>
+      <c r="M21" s="46"/>
+      <c r="N21" s="46"/>
+      <c r="O21" s="46"/>
+      <c r="P21" s="46"/>
+      <c r="R21" s="47">
+        <f>SUM(R19:S19)</f>
+        <v>0</v>
+      </c>
+      <c r="S21" s="47"/>
+      <c r="T21" s="48">
+        <f>SUM(T19+V19)</f>
+        <v>7</v>
+      </c>
+      <c r="U21" s="48"/>
+      <c r="V21" s="49">
+        <f>SUM(U19+W19)</f>
+        <v>0</v>
+      </c>
+      <c r="W21" s="49"/>
+    </row>
+    <row r="22" spans="1:24" customHeight="1" ht="19.5">
+      <c r="B22" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="40"/>
+      <c r="D22" s="41">
+        <f>K19</f>
+        <v>0</v>
+      </c>
+      <c r="E22" s="42"/>
+      <c r="J22" s="44"/>
+      <c r="K22" s="44"/>
+      <c r="L22" s="46"/>
+      <c r="M22" s="46"/>
+      <c r="N22" s="46"/>
+      <c r="O22" s="46"/>
+      <c r="P22" s="46"/>
+      <c r="R22" s="47"/>
+      <c r="S22" s="47"/>
+      <c r="T22" s="48"/>
+      <c r="U22" s="48"/>
+      <c r="V22" s="49"/>
+      <c r="W22" s="49"/>
+    </row>
+    <row r="23" spans="1:24" customHeight="1" ht="19.5">
+      <c r="B23" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="40"/>
+      <c r="D23" s="41">
+        <f>D21-D22</f>
+        <v>1050</v>
+      </c>
+      <c r="E23" s="42"/>
+      <c r="T23" s="43">
+        <f>SUM(T21:W22)</f>
+        <v>7</v>
+      </c>
+      <c r="U23" s="43"/>
+      <c r="V23" s="43"/>
+      <c r="W23" s="43"/>
+    </row>
+    <row r="24" spans="1:24" customHeight="1" ht="19.5">
+      <c r="N24" s="50">
+        <f>SUM(Q19+K19)</f>
+        <v>0</v>
+      </c>
+      <c r="O24" s="51"/>
+      <c r="T24" s="43"/>
+      <c r="U24" s="43"/>
+      <c r="V24" s="43"/>
+      <c r="W24" s="43"/>
+    </row>
+    <row r="25" spans="1:24" customHeight="1" ht="19.5">
+      <c r="I25" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="J25" s="53">
+        <f>SUM(D20-N24)</f>
+        <v>1050</v>
+      </c>
+      <c r="N25" s="51"/>
+      <c r="O25" s="51"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
@@ -1738,21 +1922,21 @@
     <mergeCell ref="V8:W8"/>
     <mergeCell ref="X7:X9"/>
     <mergeCell ref="B10:C11"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="J17:K18"/>
-    <mergeCell ref="L17:P18"/>
-    <mergeCell ref="R17:S18"/>
-    <mergeCell ref="T17:U18"/>
-    <mergeCell ref="V17:W18"/>
-    <mergeCell ref="T19:W20"/>
-    <mergeCell ref="N20:O21"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="J21:K22"/>
+    <mergeCell ref="L21:P22"/>
+    <mergeCell ref="R21:S22"/>
+    <mergeCell ref="T21:U22"/>
+    <mergeCell ref="V21:W22"/>
+    <mergeCell ref="T23:W24"/>
+    <mergeCell ref="N24:O25"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
details fin de projet
</commit_message>
<xml_diff>
--- a/src/fichiers/csv_adherents/adherents.xlsx
+++ b/src/fichiers/csv_adherents/adherents.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="45">
   <si>
     <t>ADHERENTS SAISON SPORTIVE 2021-2022</t>
   </si>
@@ -122,46 +122,16 @@
     <t>Exemple, ne rien écrire dans ces 2 lignes et ne pas les supprimer</t>
   </si>
   <si>
-    <t>DJAHNIT</t>
-  </si>
-  <si>
-    <t>Yanis</t>
-  </si>
-  <si>
-    <t>fedrgetgd</t>
-  </si>
-  <si>
-    <t>gsdzfgrezfs</t>
-  </si>
-  <si>
-    <t>fg</t>
-  </si>
-  <si>
-    <t>rerthsgthr</t>
-  </si>
-  <si>
-    <t>gsrefgfsrfg</t>
-  </si>
-  <si>
-    <t>gq</t>
-  </si>
-  <si>
-    <t>sdivhdsiof</t>
-  </si>
-  <si>
-    <t>sdifndsif</t>
-  </si>
-  <si>
-    <t>io</t>
+    <t>okkk</t>
+  </si>
+  <si>
+    <t>ihd</t>
+  </si>
+  <si>
+    <t>yanis</t>
   </si>
   <si>
     <t>djahit</t>
-  </si>
-  <si>
-    <t>ihd</t>
-  </si>
-  <si>
-    <t>okkk</t>
   </si>
   <si>
     <t>Total</t>
@@ -974,10 +944,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:X25"/>
+  <dimension ref="A1:X21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="W19" sqref="W19"/>
+      <selection activeCell="W15" sqref="W15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="true" defaultRowHeight="22.5" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1431,11 +1401,11 @@
       <c r="Q12" s="22"/>
       <c r="R12" s="20"/>
       <c r="S12" s="21"/>
-      <c r="T12" s="23"/>
+      <c r="T12" s="23">
+        <v>1</v>
+      </c>
       <c r="U12" s="24"/>
-      <c r="V12" s="25">
-        <v>1</v>
-      </c>
+      <c r="V12" s="25"/>
       <c r="W12" s="26"/>
       <c r="X12" s="8"/>
     </row>
@@ -1447,7 +1417,7 @@
         <v>37</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D13" s="20">
         <v>0</v>
@@ -1456,13 +1426,11 @@
         <f>E11</f>
         <v>150</v>
       </c>
-      <c r="F13" s="18"/>
-      <c r="G13" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="H13" s="19">
+      <c r="F13" s="18">
         <v>1</v>
       </c>
+      <c r="G13" s="8"/>
+      <c r="H13" s="19"/>
       <c r="I13" s="20"/>
       <c r="J13" s="17"/>
       <c r="K13" s="14"/>
@@ -1474,23 +1442,23 @@
       <c r="Q13" s="22"/>
       <c r="R13" s="20"/>
       <c r="S13" s="21"/>
-      <c r="T13" s="23">
+      <c r="T13" s="23"/>
+      <c r="U13" s="24"/>
+      <c r="V13" s="25">
         <v>1</v>
       </c>
-      <c r="U13" s="24"/>
-      <c r="V13" s="25"/>
       <c r="W13" s="26"/>
       <c r="X13" s="8"/>
     </row>
     <row r="14" spans="1:24">
-      <c r="A14" s="8">
+      <c r="A14" s="27">
         <v>3</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D14" s="20">
         <v>0</v>
@@ -1500,8 +1468,8 @@
         <v>150</v>
       </c>
       <c r="F14" s="18"/>
-      <c r="G14" s="8" t="s">
-        <v>42</v>
+      <c r="G14" s="8">
+        <v>54</v>
       </c>
       <c r="H14" s="19">
         <v>1</v>
@@ -1517,376 +1485,210 @@
       <c r="Q14" s="22"/>
       <c r="R14" s="20"/>
       <c r="S14" s="21"/>
-      <c r="T14" s="23">
+      <c r="T14" s="23"/>
+      <c r="U14" s="24"/>
+      <c r="V14" s="25">
         <v>1</v>
       </c>
-      <c r="U14" s="24"/>
-      <c r="V14" s="25"/>
       <c r="W14" s="26"/>
       <c r="X14" s="8"/>
     </row>
-    <row r="15" spans="1:24">
-      <c r="A15" s="8">
-        <v>4</v>
-      </c>
-      <c r="B15" s="18" t="s">
+    <row r="15" spans="1:24" customHeight="1" ht="30">
+      <c r="B15" s="54"/>
+      <c r="C15" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="30">
+        <f>SUM(D12:D14)</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="30">
+        <f>SUM(E12:E14)</f>
+        <v>450</v>
+      </c>
+      <c r="F15" s="28">
+        <f>SUM(F12:F14)</f>
+        <v>2</v>
+      </c>
+      <c r="G15" s="31"/>
+      <c r="H15" s="28">
+        <f>SUM(H12:H14)</f>
+        <v>1</v>
+      </c>
+      <c r="I15" s="30">
+        <f>SUM(I12:I14)</f>
+        <v>0</v>
+      </c>
+      <c r="J15" s="30">
+        <f>SUM(J12:J14)</f>
+        <v>0</v>
+      </c>
+      <c r="K15" s="32">
+        <f>SUM(K12:K14)</f>
+        <v>0</v>
+      </c>
+      <c r="L15" s="30">
+        <f>SUM(L12:L14)</f>
+        <v>0</v>
+      </c>
+      <c r="M15" s="29">
+        <f>SUM(M12:M14)</f>
+        <v>0</v>
+      </c>
+      <c r="N15" s="29">
+        <f>SUM(N12:N14)</f>
+        <v>0</v>
+      </c>
+      <c r="O15" s="29">
+        <f>SUM(O12:O14)</f>
+        <v>0</v>
+      </c>
+      <c r="P15" s="29">
+        <f>SUM(P12:P14)</f>
+        <v>0</v>
+      </c>
+      <c r="Q15" s="32">
+        <f>SUM(Q12:Q14)</f>
+        <v>0</v>
+      </c>
+      <c r="R15" s="33">
+        <f>SUM(R12:R14)</f>
+        <v>0</v>
+      </c>
+      <c r="S15" s="33">
+        <f>SUM(S12:S14)</f>
+        <v>0</v>
+      </c>
+      <c r="T15" s="34">
+        <f>SUM(T12:T14)</f>
+        <v>1</v>
+      </c>
+      <c r="U15" s="35">
+        <f>SUM(U12:U14)</f>
+        <v>0</v>
+      </c>
+      <c r="V15" s="34">
+        <f>SUM(V12:V14)</f>
+        <v>2</v>
+      </c>
+      <c r="W15" s="55">
+        <f>SUM(W12:W14)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" customHeight="1" ht="30">
+      <c r="D16" s="36">
+        <f>SUM(D15:E15)</f>
+        <v>450</v>
+      </c>
+      <c r="E16" s="37"/>
+      <c r="O16" s="38">
+        <f>SUM(O15:P15)</f>
+        <v>0</v>
+      </c>
+      <c r="P16" s="37"/>
+    </row>
+    <row r="17" spans="1:24" customHeight="1" ht="19.5">
+      <c r="B17" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="40"/>
+      <c r="D17" s="41">
+        <f>D16</f>
+        <v>450</v>
+      </c>
+      <c r="E17" s="42"/>
+      <c r="J17" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="K17" s="44"/>
+      <c r="L17" s="45">
+        <f>SUM(L15:P15)</f>
+        <v>0</v>
+      </c>
+      <c r="M17" s="46"/>
+      <c r="N17" s="46"/>
+      <c r="O17" s="46"/>
+      <c r="P17" s="46"/>
+      <c r="R17" s="47">
+        <f>SUM(R15:S15)</f>
+        <v>0</v>
+      </c>
+      <c r="S17" s="47"/>
+      <c r="T17" s="48">
+        <f>SUM(T15+V15)</f>
+        <v>3</v>
+      </c>
+      <c r="U17" s="48"/>
+      <c r="V17" s="49">
+        <f>SUM(U15+W15)</f>
+        <v>0</v>
+      </c>
+      <c r="W17" s="49"/>
+    </row>
+    <row r="18" spans="1:24" customHeight="1" ht="19.5">
+      <c r="B18" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="40"/>
+      <c r="D18" s="41">
+        <f>K15</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="42"/>
+      <c r="J18" s="44"/>
+      <c r="K18" s="44"/>
+      <c r="L18" s="46"/>
+      <c r="M18" s="46"/>
+      <c r="N18" s="46"/>
+      <c r="O18" s="46"/>
+      <c r="P18" s="46"/>
+      <c r="R18" s="47"/>
+      <c r="S18" s="47"/>
+      <c r="T18" s="48"/>
+      <c r="U18" s="48"/>
+      <c r="V18" s="49"/>
+      <c r="W18" s="49"/>
+    </row>
+    <row r="19" spans="1:24" customHeight="1" ht="19.5">
+      <c r="B19" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="40"/>
+      <c r="D19" s="41">
+        <f>D17-D18</f>
+        <v>450</v>
+      </c>
+      <c r="E19" s="42"/>
+      <c r="T19" s="43">
+        <f>SUM(T17:W18)</f>
+        <v>3</v>
+      </c>
+      <c r="U19" s="43"/>
+      <c r="V19" s="43"/>
+      <c r="W19" s="43"/>
+    </row>
+    <row r="20" spans="1:24" customHeight="1" ht="19.5">
+      <c r="N20" s="50">
+        <f>SUM(Q15+K15)</f>
+        <v>0</v>
+      </c>
+      <c r="O20" s="51"/>
+      <c r="T20" s="43"/>
+      <c r="U20" s="43"/>
+      <c r="V20" s="43"/>
+      <c r="W20" s="43"/>
+    </row>
+    <row r="21" spans="1:24" customHeight="1" ht="19.5">
+      <c r="I21" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="20">
-        <v>0</v>
-      </c>
-      <c r="E15" s="21">
-        <f>E11</f>
-        <v>150</v>
-      </c>
-      <c r="F15" s="18"/>
-      <c r="G15" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="H15" s="19">
-        <v>1</v>
-      </c>
-      <c r="I15" s="20"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="20"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="17"/>
-      <c r="O15" s="17"/>
-      <c r="P15" s="21"/>
-      <c r="Q15" s="22"/>
-      <c r="R15" s="20"/>
-      <c r="S15" s="21"/>
-      <c r="T15" s="23">
-        <v>1</v>
-      </c>
-      <c r="U15" s="24"/>
-      <c r="V15" s="25"/>
-      <c r="W15" s="26"/>
-      <c r="X15" s="8"/>
-    </row>
-    <row r="16" spans="1:24">
-      <c r="A16" s="8">
-        <v>5</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" s="20">
-        <v>0</v>
-      </c>
-      <c r="E16" s="21">
-        <f>E11</f>
-        <v>150</v>
-      </c>
-      <c r="F16" s="18">
-        <v>1</v>
-      </c>
-      <c r="G16" s="8"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="20"/>
-      <c r="M16" s="17"/>
-      <c r="N16" s="17"/>
-      <c r="O16" s="17"/>
-      <c r="P16" s="21"/>
-      <c r="Q16" s="22"/>
-      <c r="R16" s="20"/>
-      <c r="S16" s="21"/>
-      <c r="T16" s="23">
-        <v>1</v>
-      </c>
-      <c r="U16" s="24"/>
-      <c r="V16" s="25"/>
-      <c r="W16" s="26"/>
-      <c r="X16" s="8"/>
-    </row>
-    <row r="17" spans="1:24">
-      <c r="A17" s="8">
-        <v>6</v>
-      </c>
-      <c r="B17" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" s="20">
-        <v>0</v>
-      </c>
-      <c r="E17" s="21">
-        <f>E11</f>
-        <v>150</v>
-      </c>
-      <c r="F17" s="18">
-        <v>1</v>
-      </c>
-      <c r="G17" s="8"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="20"/>
-      <c r="M17" s="17"/>
-      <c r="N17" s="17"/>
-      <c r="O17" s="17"/>
-      <c r="P17" s="21"/>
-      <c r="Q17" s="22"/>
-      <c r="R17" s="20"/>
-      <c r="S17" s="21"/>
-      <c r="T17" s="23">
-        <v>1</v>
-      </c>
-      <c r="U17" s="24"/>
-      <c r="V17" s="25"/>
-      <c r="W17" s="26"/>
-      <c r="X17" s="8"/>
-    </row>
-    <row r="18" spans="1:24">
-      <c r="A18" s="27">
-        <v>7</v>
-      </c>
-      <c r="B18" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" s="20">
-        <v>0</v>
-      </c>
-      <c r="E18" s="21">
-        <f>E11</f>
-        <v>150</v>
-      </c>
-      <c r="F18" s="18">
-        <v>1</v>
-      </c>
-      <c r="G18" s="8"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="20"/>
-      <c r="M18" s="17"/>
-      <c r="N18" s="17"/>
-      <c r="O18" s="17"/>
-      <c r="P18" s="21"/>
-      <c r="Q18" s="22"/>
-      <c r="R18" s="20"/>
-      <c r="S18" s="21"/>
-      <c r="T18" s="23">
-        <v>1</v>
-      </c>
-      <c r="U18" s="24"/>
-      <c r="V18" s="25"/>
-      <c r="W18" s="26"/>
-      <c r="X18" s="8"/>
-    </row>
-    <row r="19" spans="1:24" customHeight="1" ht="30">
-      <c r="B19" s="54"/>
-      <c r="C19" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="D19" s="30">
-        <f>SUM(D12:D18)</f>
-        <v>0</v>
-      </c>
-      <c r="E19" s="30">
-        <f>SUM(E12:E18)</f>
-        <v>1050</v>
-      </c>
-      <c r="F19" s="28">
-        <f>SUM(F12:F18)</f>
-        <v>4</v>
-      </c>
-      <c r="G19" s="31"/>
-      <c r="H19" s="28">
-        <f>SUM(H12:H18)</f>
-        <v>3</v>
-      </c>
-      <c r="I19" s="30">
-        <f>SUM(I12:I18)</f>
-        <v>0</v>
-      </c>
-      <c r="J19" s="30">
-        <f>SUM(J12:J18)</f>
-        <v>0</v>
-      </c>
-      <c r="K19" s="32">
-        <f>SUM(K12:K18)</f>
-        <v>0</v>
-      </c>
-      <c r="L19" s="30">
-        <f>SUM(L12:L18)</f>
-        <v>0</v>
-      </c>
-      <c r="M19" s="29">
-        <f>SUM(M12:M18)</f>
-        <v>0</v>
-      </c>
-      <c r="N19" s="29">
-        <f>SUM(N12:N18)</f>
-        <v>0</v>
-      </c>
-      <c r="O19" s="29">
-        <f>SUM(O12:O18)</f>
-        <v>0</v>
-      </c>
-      <c r="P19" s="29">
-        <f>SUM(P12:P18)</f>
-        <v>0</v>
-      </c>
-      <c r="Q19" s="32">
-        <f>SUM(Q12:Q18)</f>
-        <v>0</v>
-      </c>
-      <c r="R19" s="33">
-        <f>SUM(R12:R18)</f>
-        <v>0</v>
-      </c>
-      <c r="S19" s="33">
-        <f>SUM(S12:S18)</f>
-        <v>0</v>
-      </c>
-      <c r="T19" s="34">
-        <f>SUM(T12:T18)</f>
-        <v>6</v>
-      </c>
-      <c r="U19" s="35">
-        <f>SUM(U12:U18)</f>
-        <v>0</v>
-      </c>
-      <c r="V19" s="34">
-        <f>SUM(V12:V18)</f>
-        <v>1</v>
-      </c>
-      <c r="W19" s="55">
-        <f>SUM(W12:W18)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:24" customHeight="1" ht="30">
-      <c r="D20" s="36">
-        <f>SUM(D19:E19)</f>
-        <v>1050</v>
-      </c>
-      <c r="E20" s="37"/>
-      <c r="O20" s="38">
-        <f>SUM(O19:P19)</f>
-        <v>0</v>
-      </c>
-      <c r="P20" s="37"/>
-    </row>
-    <row r="21" spans="1:24" customHeight="1" ht="19.5">
-      <c r="B21" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="C21" s="40"/>
-      <c r="D21" s="41">
-        <f>D20</f>
-        <v>1050</v>
-      </c>
-      <c r="E21" s="42"/>
-      <c r="J21" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="K21" s="44"/>
-      <c r="L21" s="45">
-        <f>SUM(L19:P19)</f>
-        <v>0</v>
-      </c>
-      <c r="M21" s="46"/>
-      <c r="N21" s="46"/>
-      <c r="O21" s="46"/>
-      <c r="P21" s="46"/>
-      <c r="R21" s="47">
-        <f>SUM(R19:S19)</f>
-        <v>0</v>
-      </c>
-      <c r="S21" s="47"/>
-      <c r="T21" s="48">
-        <f>SUM(T19+V19)</f>
-        <v>7</v>
-      </c>
-      <c r="U21" s="48"/>
-      <c r="V21" s="49">
-        <f>SUM(U19+W19)</f>
-        <v>0</v>
-      </c>
-      <c r="W21" s="49"/>
-    </row>
-    <row r="22" spans="1:24" customHeight="1" ht="19.5">
-      <c r="B22" s="39" t="s">
-        <v>51</v>
-      </c>
-      <c r="C22" s="40"/>
-      <c r="D22" s="41">
-        <f>K19</f>
-        <v>0</v>
-      </c>
-      <c r="E22" s="42"/>
-      <c r="J22" s="44"/>
-      <c r="K22" s="44"/>
-      <c r="L22" s="46"/>
-      <c r="M22" s="46"/>
-      <c r="N22" s="46"/>
-      <c r="O22" s="46"/>
-      <c r="P22" s="46"/>
-      <c r="R22" s="47"/>
-      <c r="S22" s="47"/>
-      <c r="T22" s="48"/>
-      <c r="U22" s="48"/>
-      <c r="V22" s="49"/>
-      <c r="W22" s="49"/>
-    </row>
-    <row r="23" spans="1:24" customHeight="1" ht="19.5">
-      <c r="B23" s="39" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" s="40"/>
-      <c r="D23" s="41">
-        <f>D21-D22</f>
-        <v>1050</v>
-      </c>
-      <c r="E23" s="42"/>
-      <c r="T23" s="43">
-        <f>SUM(T21:W22)</f>
-        <v>7</v>
-      </c>
-      <c r="U23" s="43"/>
-      <c r="V23" s="43"/>
-      <c r="W23" s="43"/>
-    </row>
-    <row r="24" spans="1:24" customHeight="1" ht="19.5">
-      <c r="N24" s="50">
-        <f>SUM(Q19+K19)</f>
-        <v>0</v>
-      </c>
-      <c r="O24" s="51"/>
-      <c r="T24" s="43"/>
-      <c r="U24" s="43"/>
-      <c r="V24" s="43"/>
-      <c r="W24" s="43"/>
-    </row>
-    <row r="25" spans="1:24" customHeight="1" ht="19.5">
-      <c r="I25" s="52" t="s">
-        <v>54</v>
-      </c>
-      <c r="J25" s="53">
-        <f>SUM(D20-N24)</f>
-        <v>1050</v>
-      </c>
-      <c r="N25" s="51"/>
-      <c r="O25" s="51"/>
+      <c r="J21" s="53">
+        <f>SUM(D16-N20)</f>
+        <v>450</v>
+      </c>
+      <c r="N21" s="51"/>
+      <c r="O21" s="51"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
@@ -1922,21 +1724,21 @@
     <mergeCell ref="V8:W8"/>
     <mergeCell ref="X7:X9"/>
     <mergeCell ref="B10:C11"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="J21:K22"/>
-    <mergeCell ref="L21:P22"/>
-    <mergeCell ref="R21:S22"/>
-    <mergeCell ref="T21:U22"/>
-    <mergeCell ref="V21:W22"/>
-    <mergeCell ref="T23:W24"/>
-    <mergeCell ref="N24:O25"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="J17:K18"/>
+    <mergeCell ref="L17:P18"/>
+    <mergeCell ref="R17:S18"/>
+    <mergeCell ref="T17:U18"/>
+    <mergeCell ref="V17:W18"/>
+    <mergeCell ref="T19:W20"/>
+    <mergeCell ref="N20:O21"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>